<commit_message>
Update 27/11/2023 - 5:19
</commit_message>
<xml_diff>
--- a/KGlob.xlsx
+++ b/KGlob.xlsx
@@ -494,7 +494,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1243.503116200358</v>
+        <v>1.243503116200358</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -521,7 +521,7 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>-1243.503116200358</v>
+        <v>-1.243503116200358</v>
       </c>
       <c r="L2" t="n">
         <v>0</v>
@@ -556,10 +556,10 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>34.54175322778771</v>
+        <v>0.03454175322778771</v>
       </c>
       <c r="D3" t="n">
-        <v>51.81262984168157</v>
+        <v>0.05181262984168157</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -583,10 +583,10 @@
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>-34.54175322778771</v>
+        <v>-0.03454175322778771</v>
       </c>
       <c r="M3" t="n">
-        <v>51.81262984168157</v>
+        <v>0.05181262984168157</v>
       </c>
       <c r="N3" t="n">
         <v>0</v>
@@ -615,10 +615,10 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>51.81262984168157</v>
+        <v>0.05181262984168157</v>
       </c>
       <c r="D4" t="n">
-        <v>103.6252596833631</v>
+        <v>0.1036252596833631</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -642,10 +642,10 @@
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>-51.81262984168157</v>
+        <v>-0.05181262984168157</v>
       </c>
       <c r="M4" t="n">
-        <v>51.81262984168157</v>
+        <v>0.05181262984168156</v>
       </c>
       <c r="N4" t="n">
         <v>0</v>
@@ -680,7 +680,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>1578.881281869028</v>
+        <v>1.578881281869029</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -689,7 +689,7 @@
         <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>-489.8398753146541</v>
+        <v>-0.4898398753146541</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -698,7 +698,7 @@
         <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>-532.9299069430105</v>
+        <v>-0.5329299069430105</v>
       </c>
       <c r="L5" t="n">
         <v>0</v>
@@ -707,7 +707,7 @@
         <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>-556.1114996113639</v>
+        <v>0</v>
       </c>
       <c r="O5" t="n">
         <v>0</v>
@@ -722,7 +722,7 @@
         <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>0</v>
+        <v>-0.556111499611364</v>
       </c>
     </row>
     <row r="6">
@@ -742,37 +742,37 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>7.919917241546575</v>
+        <v>0.007919917241546575</v>
       </c>
       <c r="G6" t="n">
-        <v>-7.193970350291183</v>
+        <v>-0.007193970350291186</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>-2.111378772907992</v>
+        <v>-0.002111378772907992</v>
       </c>
       <c r="J6" t="n">
-        <v>-8.039890837502311</v>
+        <v>-0.008039890837502311</v>
       </c>
       <c r="K6" t="n">
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>-2.719030137464339</v>
+        <v>-0.002719030137464339</v>
       </c>
       <c r="M6" t="n">
-        <v>-9.516605481125186</v>
+        <v>-0.009516605481125186</v>
       </c>
       <c r="N6" t="n">
         <v>0</v>
       </c>
       <c r="O6" t="n">
-        <v>-3.089508331174244</v>
+        <v>-0.003089508331174243</v>
       </c>
       <c r="P6" t="n">
-        <v>10.36252596833631</v>
+        <v>0.01036252596833631</v>
       </c>
       <c r="Q6" t="n">
         <v>0</v>
@@ -801,37 +801,37 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>-7.193970350291183</v>
+        <v>-0.007193970350291186</v>
       </c>
       <c r="G7" t="n">
-        <v>131.5734401557524</v>
+        <v>0.1315734401557524</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>8.039890837502311</v>
+        <v>0.008039890837502311</v>
       </c>
       <c r="J7" t="n">
-        <v>20.40999480477726</v>
+        <v>0.02040999480477725</v>
       </c>
       <c r="K7" t="n">
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>9.516605481125186</v>
+        <v>0.009516605481125186</v>
       </c>
       <c r="M7" t="n">
-        <v>22.2054127892921</v>
+        <v>0.0222054127892921</v>
       </c>
       <c r="N7" t="n">
         <v>0</v>
       </c>
       <c r="O7" t="n">
-        <v>-10.36252596833631</v>
+        <v>-0.01036252596833631</v>
       </c>
       <c r="P7" t="n">
-        <v>23.17131248380683</v>
+        <v>0.02317131248380683</v>
       </c>
       <c r="Q7" t="n">
         <v>0</v>
@@ -857,7 +857,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>-489.8398753146541</v>
+        <v>-0.4898398753146541</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -866,7 +866,7 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>1535.160290982592</v>
+        <v>1.535160290982592</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -875,7 +875,7 @@
         <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>-462.712736936295</v>
+        <v>-0.4627127369362951</v>
       </c>
       <c r="L8" t="n">
         <v>0</v>
@@ -893,7 +893,7 @@
         <v>0</v>
       </c>
       <c r="Q8" t="n">
-        <v>-582.6076787316429</v>
+        <v>-0.5826076787316429</v>
       </c>
       <c r="R8" t="n">
         <v>0</v>
@@ -919,31 +919,31 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>-2.111378772907992</v>
+        <v>-0.002111378772907992</v>
       </c>
       <c r="G9" t="n">
-        <v>8.039890837502311</v>
+        <v>0.008039890837502311</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>7.443528991664547</v>
+        <v>0.007443528991664547</v>
       </c>
       <c r="J9" t="n">
-        <v>12.2393385094735</v>
+        <v>0.0122393385094735</v>
       </c>
       <c r="K9" t="n">
         <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>-1.779664372831904</v>
+        <v>-0.001779664372831904</v>
       </c>
       <c r="M9" t="n">
-        <v>-7.174056439617449</v>
+        <v>-0.00717405643961745</v>
       </c>
       <c r="N9" t="n">
-        <v>0</v>
+        <v>0.01137350411158864</v>
       </c>
       <c r="O9" t="n">
         <v>0</v>
@@ -955,10 +955,10 @@
         <v>0</v>
       </c>
       <c r="R9" t="n">
-        <v>-3.552485845924652</v>
+        <v>-0.003552485845924652</v>
       </c>
       <c r="S9" t="n">
-        <v>11.37350411158864</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -978,31 +978,31 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>-8.039890837502311</v>
+        <v>-0.008039890837502311</v>
       </c>
       <c r="G10" t="n">
-        <v>20.40999480477726</v>
+        <v>0.02040999480477725</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>12.2393385094735</v>
+        <v>0.0122393385094735</v>
       </c>
       <c r="J10" t="n">
-        <v>127.9300242485493</v>
+        <v>0.1279300242485493</v>
       </c>
       <c r="K10" t="n">
         <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>7.174056439617449</v>
+        <v>0.00717405643961745</v>
       </c>
       <c r="M10" t="n">
-        <v>19.27969737234563</v>
+        <v>0.01927969737234562</v>
       </c>
       <c r="N10" t="n">
-        <v>0</v>
+        <v>0.02427531994715179</v>
       </c>
       <c r="O10" t="n">
         <v>0</v>
@@ -1014,10 +1014,10 @@
         <v>0</v>
       </c>
       <c r="R10" t="n">
-        <v>-11.37350411158864</v>
+        <v>-0.01137350411158864</v>
       </c>
       <c r="S10" t="n">
-        <v>24.27531994715179</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -1025,7 +1025,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>-1243.503116200358</v>
+        <v>-1.243503116200358</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
@@ -1034,7 +1034,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>-532.9299069430105</v>
+        <v>-0.5329299069430105</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -1043,7 +1043,7 @@
         <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>-462.712736936295</v>
+        <v>-0.4627127369362951</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
@@ -1052,7 +1052,7 @@
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>2239.145760079663</v>
+        <v>2.239145760079663</v>
       </c>
       <c r="L11" t="n">
         <v>0</v>
@@ -1087,37 +1087,37 @@
         <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>-34.54175322778771</v>
+        <v>-0.03454175322778771</v>
       </c>
       <c r="D12" t="n">
-        <v>-51.81262984168157</v>
+        <v>-0.05181262984168157</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>-2.719030137464339</v>
+        <v>-0.002719030137464339</v>
       </c>
       <c r="G12" t="n">
-        <v>9.516605481125186</v>
+        <v>0.009516605481125186</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>-1.779664372831904</v>
+        <v>-0.001779664372831904</v>
       </c>
       <c r="J12" t="n">
-        <v>7.174056439617449</v>
+        <v>0.00717405643961745</v>
       </c>
       <c r="K12" t="n">
         <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>39.04044773808395</v>
+        <v>0.03904044773808395</v>
       </c>
       <c r="M12" t="n">
-        <v>-35.12196792093893</v>
+        <v>-0.03512196792093893</v>
       </c>
       <c r="N12" t="n">
         <v>0</v>
@@ -1146,37 +1146,37 @@
         <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>51.81262984168157</v>
+        <v>0.05181262984168157</v>
       </c>
       <c r="D13" t="n">
-        <v>51.81262984168157</v>
+        <v>0.05181262984168156</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>-9.516605481125186</v>
+        <v>-0.009516605481125186</v>
       </c>
       <c r="G13" t="n">
-        <v>22.2054127892921</v>
+        <v>0.0222054127892921</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>-7.174056439617449</v>
+        <v>-0.00717405643961745</v>
       </c>
       <c r="J13" t="n">
-        <v>19.27969737234563</v>
+        <v>0.01927969737234562</v>
       </c>
       <c r="K13" t="n">
         <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>-35.12196792093893</v>
+        <v>-0.03512196792093893</v>
       </c>
       <c r="M13" t="n">
-        <v>186.5954800066386</v>
+        <v>0.1865954800066386</v>
       </c>
       <c r="N13" t="n">
         <v>0</v>
@@ -1211,7 +1211,7 @@
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>-556.1114996113639</v>
+        <v>0</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -1223,10 +1223,10 @@
         <v>0</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>0.01137350411158864</v>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>0.02427531994715179</v>
       </c>
       <c r="K14" t="n">
         <v>0</v>
@@ -1238,7 +1238,7 @@
         <v>0</v>
       </c>
       <c r="N14" t="n">
-        <v>556.1114996113639</v>
+        <v>0.04855063989430358</v>
       </c>
       <c r="O14" t="n">
         <v>0</v>
@@ -1250,7 +1250,7 @@
         <v>0</v>
       </c>
       <c r="R14" t="n">
-        <v>0</v>
+        <v>-0.01137350411158864</v>
       </c>
       <c r="S14" t="n">
         <v>0</v>
@@ -1273,10 +1273,10 @@
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>-3.089508331174244</v>
+        <v>-0.003089508331174243</v>
       </c>
       <c r="G15" t="n">
-        <v>-10.36252596833631</v>
+        <v>-0.01036252596833631</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -1300,10 +1300,10 @@
         <v>0</v>
       </c>
       <c r="O15" t="n">
-        <v>3.089508331174244</v>
+        <v>0.003089508331174243</v>
       </c>
       <c r="P15" t="n">
-        <v>-10.36252596833631</v>
+        <v>-0.01036252596833631</v>
       </c>
       <c r="Q15" t="n">
         <v>0</v>
@@ -1332,10 +1332,10 @@
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>10.36252596833631</v>
+        <v>0.01036252596833631</v>
       </c>
       <c r="G16" t="n">
-        <v>23.17131248380683</v>
+        <v>0.02317131248380683</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -1359,10 +1359,10 @@
         <v>0</v>
       </c>
       <c r="O16" t="n">
-        <v>-10.36252596833631</v>
+        <v>-0.01036252596833631</v>
       </c>
       <c r="P16" t="n">
-        <v>46.34262496761366</v>
+        <v>0.04634262496761365</v>
       </c>
       <c r="Q16" t="n">
         <v>0</v>
@@ -1397,7 +1397,7 @@
         <v>0</v>
       </c>
       <c r="H17" t="n">
-        <v>-582.6076787316429</v>
+        <v>-0.5826076787316429</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
@@ -1424,7 +1424,7 @@
         <v>0</v>
       </c>
       <c r="Q17" t="n">
-        <v>582.6076787316429</v>
+        <v>0.5826076787316429</v>
       </c>
       <c r="R17" t="n">
         <v>0</v>
@@ -1459,10 +1459,10 @@
         <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>-3.552485845924652</v>
+        <v>-0.003552485845924652</v>
       </c>
       <c r="J18" t="n">
-        <v>-11.37350411158864</v>
+        <v>-0.01137350411158864</v>
       </c>
       <c r="K18" t="n">
         <v>0</v>
@@ -1474,7 +1474,7 @@
         <v>0</v>
       </c>
       <c r="N18" t="n">
-        <v>0</v>
+        <v>-0.01137350411158864</v>
       </c>
       <c r="O18" t="n">
         <v>0</v>
@@ -1486,10 +1486,10 @@
         <v>0</v>
       </c>
       <c r="R18" t="n">
-        <v>3.552485845924652</v>
+        <v>0.003552485845924652</v>
       </c>
       <c r="S18" t="n">
-        <v>-11.37350411158864</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1506,7 +1506,7 @@
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>-0.556111499611364</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -1518,10 +1518,10 @@
         <v>0</v>
       </c>
       <c r="I19" t="n">
-        <v>11.37350411158864</v>
+        <v>0</v>
       </c>
       <c r="J19" t="n">
-        <v>24.27531994715179</v>
+        <v>0</v>
       </c>
       <c r="K19" t="n">
         <v>0</v>
@@ -1545,10 +1545,10 @@
         <v>0</v>
       </c>
       <c r="R19" t="n">
-        <v>-11.37350411158864</v>
+        <v>0</v>
       </c>
       <c r="S19" t="n">
-        <v>48.55063989430358</v>
+        <v>0.556111499611364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>